<commit_message>
muestras actualizadas. matriz 1-1-3
</commit_message>
<xml_diff>
--- a/muestras/1/workbook.xlsx
+++ b/muestras/1/workbook.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="7" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15540" tabRatio="959" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Criterios" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="ProyVsIE" sheetId="3" r:id="rId18"/>
     <sheet name="ProyVsGI" sheetId="21" r:id="rId19"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="27">
   <si>
     <t>FE</t>
   </si>
@@ -113,12 +113,18 @@
   <si>
     <t>GC</t>
   </si>
+  <si>
+    <t>Revisar tambien criterios ppal</t>
+  </si>
+  <si>
+    <t>Validado con EC al 27/07/15 y ápendices</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -164,6 +170,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -719,7 +732,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -854,12 +867,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -883,6 +890,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="147">
@@ -1036,6 +1052,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1361,10 +1382,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="6"/>
+  </sheetPr>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1374,11 +1398,11 @@
     <col min="4" max="4" width="6" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" customWidth="1"/>
     <col min="6" max="6" width="6.5" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" thickBot="1">
+    <row r="1" spans="1:7" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1388,14 +1412,14 @@
       <c r="C1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="49" t="s">
+      <c r="E1" s="58" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2" s="45" t="s">
         <v>21</v>
       </c>
@@ -1403,7 +1427,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="20">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="D2" s="20">
         <v>0.14285714285714285</v>
@@ -1412,7 +1436,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3" s="46" t="s">
         <v>5</v>
       </c>
@@ -1428,7 +1452,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7">
       <c r="A4" s="46" t="s">
         <v>6</v>
       </c>
@@ -1441,7 +1465,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16" thickBot="1">
+    <row r="5" spans="1:7" ht="16" thickBot="1">
       <c r="A5" s="47" t="s">
         <v>22</v>
       </c>
@@ -1452,12 +1476,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="G7" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1991,10 +2020,13 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <sheetPr enableFormatConditionsCalculation="0">
+    <tabColor theme="6"/>
+  </sheetPr>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2009,7 +2041,7 @@
     <col min="16" max="16" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1">
+    <row r="1" spans="1:8" ht="16" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -2029,7 +2061,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:8">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -2040,7 +2072,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="20">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="21">
         <v>5</v>
@@ -2049,7 +2081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -2063,11 +2095,11 @@
       <c r="E3" s="23">
         <v>7</v>
       </c>
-      <c r="F3" s="23">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="F3" s="56">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
@@ -2083,7 +2115,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:8">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -2094,10 +2126,10 @@
         <v>1</v>
       </c>
       <c r="F5" s="23">
-        <v>0.14285714285714285</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" s="33" t="s">
         <v>19</v>
       </c>
@@ -2107,6 +2139,11 @@
       <c r="E6" s="18"/>
       <c r="F6" s="25">
         <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="H9" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2125,13 +2162,14 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.1640625" customWidth="1"/>
-    <col min="2" max="10" width="5.83203125" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="10" width="5.83203125" customWidth="1"/>
     <col min="11" max="11" width="7.83203125" customWidth="1"/>
     <col min="12" max="13" width="6.5" customWidth="1"/>
     <col min="14" max="14" width="7.1640625" customWidth="1"/>
@@ -2278,7 +2316,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -2468,10 +2506,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16" thickBot="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="55" t="s">
         <v>15</v>
       </c>
       <c r="C1" s="31" t="s">
@@ -2488,22 +2526,22 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="51">
-        <v>1</v>
-      </c>
-      <c r="C2" s="52">
-        <v>3</v>
-      </c>
-      <c r="D2" s="52">
+      <c r="B2" s="49">
+        <v>1</v>
+      </c>
+      <c r="C2" s="50">
+        <v>3</v>
+      </c>
+      <c r="D2" s="50">
         <v>5</v>
       </c>
-      <c r="E2" s="53">
+      <c r="E2" s="51">
         <v>7</v>
       </c>
-      <c r="F2" s="53">
+      <c r="F2" s="51">
         <v>0.33333333333333331</v>
       </c>
     </row>
@@ -2556,14 +2594,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" thickBot="1">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="56">
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="54">
         <v>1</v>
       </c>
     </row>
@@ -2853,7 +2891,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3113,7 +3151,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3185,7 +3223,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="23">
-        <v>0.33333333333333331</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -3445,22 +3483,22 @@
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="48" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="51">
-        <v>1</v>
-      </c>
-      <c r="C2" s="52">
+      <c r="B2" s="49">
+        <v>1</v>
+      </c>
+      <c r="C2" s="50">
         <v>5</v>
       </c>
-      <c r="D2" s="52">
-        <v>3</v>
-      </c>
-      <c r="E2" s="53">
+      <c r="D2" s="50">
+        <v>3</v>
+      </c>
+      <c r="E2" s="51">
         <v>7</v>
       </c>
-      <c r="F2" s="53">
+      <c r="F2" s="51">
         <v>3</v>
       </c>
     </row>
@@ -3513,14 +3551,14 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="16" thickBot="1">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="56">
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="54">
         <v>1</v>
       </c>
     </row>
@@ -3795,7 +3833,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>

</xml_diff>